<commit_message>
20180622 push from pc1
</commit_message>
<xml_diff>
--- a/FAE项目问题更新-杨胜齐.xlsx
+++ b/FAE项目问题更新-杨胜齐.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Remark" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
   <si>
     <t xml:space="preserve">问题类型：</t>
   </si>
@@ -348,11 +348,38 @@
     <t xml:space="preserve">释放6M TEE OS</t>
   </si>
   <si>
+    <t xml:space="preserve">Y839</t>
+  </si>
+  <si>
     <t xml:space="preserve">1.sdrpmb写保护，写不进去key
 2.写key后固件升级key丢失</t>
   </si>
   <si>
     <t xml:space="preserve">委哥和梁总解决</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y393B11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.更换小内存版本
+2.更新小内存版本后不能开机</t>
+  </si>
+  <si>
+    <t xml:space="preserve">释放6M TEE OS,custom/build/project/工程名.mk没有修改</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y833A7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.要求更换小内存版本
+2.不能写号</t>
+  </si>
+  <si>
+    <t xml:space="preserve">释放6M TEE OS，使用工具在windows下分解的array.c格式有问题，导致
+Kph ta编译失败</t>
   </si>
   <si>
     <t xml:space="preserve">3643_LF708_navitel</t>
@@ -436,6 +463,21 @@
   </si>
   <si>
     <t xml:space="preserve">更换证书类型，更换密钥</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c509-7151h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tkcoreos 跳转地址不对</t>
+  </si>
+  <si>
+    <t xml:space="preserve">更新了tz_init.c和tz_tkcore.h，设置启动地址自动跳转</t>
+  </si>
+  <si>
+    <t xml:space="preserve">指纹不能使用，指纹读不到chip id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">修改了spi.c，更换指纹秘钥重新签名</t>
   </si>
   <si>
     <t xml:space="preserve">5025PH,5301PH,
@@ -677,14 +719,11 @@
   </sheetPr>
   <dimension ref="B4:B25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2"/>
-  </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
@@ -800,18 +839,17 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.1813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,7 +877,7 @@
     </row>
     <row r="2" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180528</v>
@@ -848,10 +886,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180528</v>
@@ -972,19 +1010,18 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.5023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.8790697674419"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.8418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.5209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1145,19 +1182,18 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.0279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.2093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.7348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.6558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,7 +1262,9 @@
       <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="45.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
+      <c r="A4" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="B4" s="6" t="n">
         <v>20180605</v>
       </c>
@@ -1234,41 +1272,77 @@
         <v>28</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>20180608</v>
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+    <row r="5" customFormat="false" ht="44.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>20180620</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>20180620</v>
+      </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+    <row r="6" customFormat="false" ht="26.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>20180619</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>20180619</v>
+      </c>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
+    <row r="7" customFormat="false" ht="47.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>20180620</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>20180921</v>
+      </c>
       <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,13 +1420,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="106.204651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="112.725581395349"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1502,18 +1575,17 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.5302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="65.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1541,7 +1613,7 @@
     </row>
     <row r="2" customFormat="false" ht="70.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180529</v>
@@ -1550,10 +1622,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180529</v>
@@ -1680,14 +1752,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.706976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.2883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1674418604651"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1715,19 +1786,19 @@
     </row>
     <row r="2" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180523</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180525</v>
@@ -1736,7 +1807,7 @@
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180530</v>
@@ -1745,10 +1816,10 @@
         <v>28</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>20180530</v>
@@ -1866,13 +1937,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.2279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.0093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.3302325581395"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.8418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.2837209302326"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,16 +1969,16 @@
     </row>
     <row r="2" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180530</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1917,7 +1986,7 @@
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180530</v>
@@ -2047,12 +2116,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="106.204651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="112.725581395349"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2201,18 +2268,17 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.9023255813954"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.7023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.6093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,19 +2306,19 @@
     </row>
     <row r="2" customFormat="false" ht="40.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180519</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180525</v>
@@ -2261,19 +2327,19 @@
     </row>
     <row r="3" customFormat="false" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180524</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>20180524</v>
@@ -2282,41 +2348,65 @@
     </row>
     <row r="4" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>20180605</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>20180605</v>
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+    <row r="5" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>20180609</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>20180611</v>
+      </c>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
+    <row r="6" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>20180621</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <v>20180621</v>
+      </c>
       <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
20180622 commit add jiangyuan y8933 and roco
</commit_message>
<xml_diff>
--- a/FAE项目问题更新-杨胜齐.xlsx
+++ b/FAE项目问题更新-杨胜齐.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Remark" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="82">
   <si>
     <t xml:space="preserve">问题类型：</t>
   </si>
@@ -382,6 +382,12 @@
 Kph ta编译失败</t>
   </si>
   <si>
+    <t xml:space="preserve">y81933</t>
+  </si>
+  <si>
+    <t xml:space="preserve">释放6M TEE OS，protect_f没有配好</t>
+  </si>
+  <si>
     <t xml:space="preserve">3643_LF708_navitel</t>
   </si>
   <si>
@@ -394,10 +400,16 @@
     <t xml:space="preserve">更换了9ef77781-****.ta</t>
   </si>
   <si>
+    <t xml:space="preserve">LF730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1开机问题</t>
+  </si>
+  <si>
+    <t xml:space="preserve">在重启测试的时候会概率性卡在logo界面开不了机</t>
+  </si>
+  <si>
     <t xml:space="preserve">V662</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1开机问题</t>
   </si>
   <si>
     <t xml:space="preserve">手机关机后可以开机，重新
@@ -724,6 +736,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86046511627907"/>
+  </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
@@ -844,12 +859,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.5162790697674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.9348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.6279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.1627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,7 +893,7 @@
     </row>
     <row r="2" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180528</v>
@@ -886,10 +902,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180528</v>
@@ -1010,18 +1026,19 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.2604651162791"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.8418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.5209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.3813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1182,18 +1199,19 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.7348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.6558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.7209302325581"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="63.5023255813954"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1341,17 +1359,29 @@
         <v>44</v>
       </c>
       <c r="F7" s="6" t="n">
-        <v>20180921</v>
+        <v>20180621</v>
       </c>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+    <row r="8" customFormat="false" ht="41.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>20180622</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="6" t="n">
+        <v>20180622</v>
+      </c>
       <c r="G8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1420,12 +1450,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="112.725581395349"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.153488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.2604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="116.172093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,17 +1606,18 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="65.2232558139535"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.1906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1613,7 +1645,7 @@
     </row>
     <row r="2" customFormat="false" ht="70.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180529</v>
@@ -1622,21 +1654,29 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180529</v>
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6"/>
+    <row r="3" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>20180622</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
@@ -1752,13 +1792,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.2883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.6418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1786,19 +1827,19 @@
     </row>
     <row r="2" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180523</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180525</v>
@@ -1807,7 +1848,7 @@
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180530</v>
@@ -1816,10 +1857,10 @@
         <v>28</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>20180530</v>
@@ -1937,11 +1978,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.2139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.8418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.2837209302326"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.3162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.8837209302326"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1969,16 +2012,16 @@
     </row>
     <row r="2" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180530</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1986,7 +2029,7 @@
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180530</v>
@@ -2116,10 +2159,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="112.725581395349"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.3674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="116.172093023256"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2274,11 +2319,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.7023255813953"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.6093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.0558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,19 +2352,19 @@
     </row>
     <row r="2" customFormat="false" ht="40.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180519</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180525</v>
@@ -2327,19 +2373,19 @@
     </row>
     <row r="3" customFormat="false" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180524</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>20180524</v>
@@ -2348,19 +2394,19 @@
     </row>
     <row r="4" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>20180605</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>20180605</v>
@@ -2369,19 +2415,19 @@
     </row>
     <row r="5" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>20180609</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>20180611</v>
@@ -2390,19 +2436,19 @@
     </row>
     <row r="6" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>20180621</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>20180621</v>

</xml_diff>

<commit_message>
add 0728 and not all a weekday
</commit_message>
<xml_diff>
--- a/FAE项目问题更新-杨胜齐.xlsx
+++ b/FAE项目问题更新-杨胜齐.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Remark" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="90">
   <si>
     <t xml:space="preserve">问题类型：</t>
   </si>
@@ -403,6 +403,15 @@
     <t xml:space="preserve">更换小内存 </t>
   </si>
   <si>
+    <t xml:space="preserve">Y30113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2指纹问题</t>
+  </si>
+  <si>
+    <t xml:space="preserve">指纹注册不到时钟</t>
+  </si>
+  <si>
     <t xml:space="preserve">3643_LF708_navitel</t>
   </si>
   <si>
@@ -485,9 +494,6 @@
   </si>
   <si>
     <t xml:space="preserve">A756-8091</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2指纹问题</t>
   </si>
   <si>
     <t xml:space="preserve">拉完代码后指纹不能用</t>
@@ -756,7 +762,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -872,19 +878,19 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="44.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.5767441860465"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,7 +918,7 @@
     </row>
     <row r="2" customFormat="false" ht="38.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180528</v>
@@ -921,10 +927,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180528</v>
@@ -1051,13 +1057,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.3627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.3162790697674"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="37.2883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1218,19 +1224,19 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.7813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="71.4976744186046"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.9953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="75.8046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1445,11 +1451,19 @@
       </c>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
+    <row r="11" customFormat="false" ht="21.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>20180725</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -1493,13 +1507,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="130.693023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="138.813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,13 +1668,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.6837209302326"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="80.2372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,7 +1702,7 @@
     </row>
     <row r="2" customFormat="false" ht="70.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180529</v>
@@ -1697,10 +1711,10 @@
         <v>32</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180529</v>
@@ -1709,19 +1723,19 @@
     </row>
     <row r="3" customFormat="false" ht="49.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180622</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>20180702</v>
@@ -1839,14 +1853,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.5348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.6232558139535"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,19 +1888,19 @@
     </row>
     <row r="2" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180523</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180525</v>
@@ -1895,7 +1909,7 @@
     </row>
     <row r="3" customFormat="false" ht="35.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180530</v>
@@ -1904,10 +1918,10 @@
         <v>28</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>20180530</v>
@@ -2025,13 +2039,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.7162790697675"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.6558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="65.3441860465116"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2059,16 +2073,16 @@
     </row>
     <row r="2" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180530</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -2076,7 +2090,7 @@
     </row>
     <row r="3" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180530</v>
@@ -2206,12 +2220,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.2279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="130.693023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.5162790697674"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="138.813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,17 +2375,17 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.2372093023256"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.6837209302326"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,19 +2413,19 @@
     </row>
     <row r="2" customFormat="false" ht="40.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B2" s="6" t="n">
         <v>20180519</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180525</v>
@@ -2420,19 +2434,19 @@
     </row>
     <row r="3" customFormat="false" ht="36.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" s="6" t="n">
         <v>20180524</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>20180524</v>
@@ -2441,19 +2455,19 @@
     </row>
     <row r="4" customFormat="false" ht="34.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B4" s="6" t="n">
         <v>20180605</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>20180605</v>
@@ -2462,19 +2476,19 @@
     </row>
     <row r="5" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B5" s="6" t="n">
         <v>20180609</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>20180611</v>
@@ -2483,19 +2497,19 @@
     </row>
     <row r="6" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B6" s="6" t="n">
         <v>20180621</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>20180621</v>

</xml_diff>

<commit_message>
add at 0824 FRI
</commit_message>
<xml_diff>
--- a/FAE项目问题更新-杨胜齐.xlsx
+++ b/FAE项目问题更新-杨胜齐.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Remark" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="160">
   <si>
     <t xml:space="preserve">问题类型：</t>
   </si>
@@ -651,6 +651,9 @@
   </si>
   <si>
     <t xml:space="preserve">现场确认是reset引脚被拉低，已经确认与tee无关</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AndroidServices没有起来，重新编译后解决</t>
   </si>
   <si>
     <t xml:space="preserve">C719-8045C</t>
@@ -902,7 +905,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,13 +1007,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.0697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.3953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.1348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.8372093023256"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.4046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.9953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1236,19 +1239,19 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.0744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="68.2976744186047"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="99.1860465116279"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.1813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.2697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="102.139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1645,13 +1648,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.7395348837209"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7162790697674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="72.353488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.3813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.6604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="74.5767441860465"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.6697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,18 +1908,18 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.246511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="89.5906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="96.3581395348837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="92.2976744186047"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="99.3116279069767"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,8 +2061,12 @@
       <c r="D7" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>20180823</v>
+      </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,19 +2138,19 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.3348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.9116279069768"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="87.4976744186047"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.153488372093"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="90.0837209302326"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,19 +2178,19 @@
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>20180519</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>20180525</v>
@@ -2192,7 +2199,7 @@
     </row>
     <row r="3" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>20180524</v>
@@ -2201,10 +2208,10 @@
         <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>20180524</v>
@@ -2213,7 +2220,7 @@
     </row>
     <row r="4" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>20180605</v>
@@ -2222,10 +2229,10 @@
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>20180605</v>
@@ -2234,7 +2241,7 @@
     </row>
     <row r="5" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>20180609</v>
@@ -2243,10 +2250,10 @@
         <v>79</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>20180611</v>
@@ -2255,7 +2262,7 @@
     </row>
     <row r="6" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>20180621</v>
@@ -2264,10 +2271,10 @@
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>20180621</v>
@@ -2276,7 +2283,7 @@
     </row>
     <row r="7" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>20180821</v>
@@ -2285,7 +2292,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2375,13 +2382,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="78.6372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="80.9767441860465"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,7 +2416,7 @@
     </row>
     <row r="2" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>20180528</v>
@@ -2418,10 +2425,10 @@
         <v>48</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>20180528</v>
@@ -2430,7 +2437,7 @@
     </row>
     <row r="3" customFormat="false" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>20180725</v>
@@ -2439,10 +2446,10 @@
         <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>20180725</v>
@@ -2554,20 +2561,20 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.8837209302326"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.2883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.1953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.846511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.9023255813953"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.353488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.6093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.8837209302326"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3348837209302"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.706976744186"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2581,7 +2588,7 @@
         <v>17</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>19</v>
@@ -2595,19 +2602,22 @@
     </row>
     <row r="2" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>20180823</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>20180824</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2617,8 +2627,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add at 0826 SUN
</commit_message>
<xml_diff>
--- a/FAE项目问题更新-杨胜齐.xlsx
+++ b/FAE项目问题更新-杨胜齐.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Remark" sheetId="1" state="visible" r:id="rId2"/>
@@ -742,7 +742,7 @@
     <t xml:space="preserve">新项目调试</t>
   </si>
   <si>
-    <t xml:space="preserve">远程调试</t>
+    <t xml:space="preserve">远程调试,pld状态，gptest，写key，otrp测试正常</t>
   </si>
 </sst>
 </file>
@@ -905,7 +905,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1007,13 +1007,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.6604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="57.8372093023256"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.4046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="55.9953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.7441860465116"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.7162790697675"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.4697674418605"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1244,14 +1244,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.1813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.7023255813953"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.1674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="70.2697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="102.139534883721"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.1627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.5674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="72.3627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="105.218604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1648,13 +1648,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.2883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.0604651162791"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="74.5767441860465"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.6697674418605"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.2744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.7813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.306976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="76.9116279069768"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.9023255813954"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1913,13 +1913,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.3348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="92.2976744186047"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="99.3116279069767"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="95.0046511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="102.26511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,19 +2138,19 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.9674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="79.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="90.0837209302326"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.7023255813953"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="81.4651162790698"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="92.7906976744186"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2382,13 +2382,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.506976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.9674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.1302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="80.9767441860465"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.4744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1209302325581"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.9488372093023"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.2232558139535"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="83.4372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2561,20 +2561,20 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.353488372093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.6093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="54.8837209302326"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.4837209302326"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.0744186046512"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2627,8 +2627,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modify chamsion fingerprint error
</commit_message>
<xml_diff>
--- a/FAE项目问题更新-杨胜齐.xlsx
+++ b/FAE项目问题更新-杨胜齐.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Remark" sheetId="1" state="visible" r:id="rId2"/>
@@ -954,9 +954,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5674418604651"/>
-  </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
@@ -1052,18 +1049,17 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.906976744186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.7674418604651"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.4372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2976744186047"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.7767441860465"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.1627906976744"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1300,19 +1296,18 @@
   </sheetPr>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.446511627907"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.4697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="82.9581395348837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.1906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.5302325581395"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="21.4139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,18 +1700,17 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.3953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.553488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.4093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.2558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.506976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.4697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.6093023255814"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1209302325581"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2017,13 +2011,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.7302325581395"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.7209302325581"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="67.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.6511627906977"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.6511627906977"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="88.2372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,19 +2242,18 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5674418604651"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="95.4976744186046"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="98.3255813953488"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6279069767442"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2398,7 +2389,7 @@
         <v>159</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>20180821</v>
+        <v>20180830</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>27</v>
@@ -2494,13 +2485,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.3488372093023"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8232558139535"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.4651162790698"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="55.7302325581395"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="83.1255813953488"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.2418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.3488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.6511627906977"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.953488372093"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2673,20 +2663,20 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.3348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.5627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.2093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.0139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.1627906976744"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.9302325581395"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.8139534883721"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2757,8 +2747,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add at 0907 FRI
</commit_message>
<xml_diff>
--- a/FAE项目问题更新-杨胜齐.xlsx
+++ b/FAE项目问题更新-杨胜齐.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Remark" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="186">
   <si>
     <t xml:space="preserve">问题类型：</t>
   </si>
@@ -387,6 +387,24 @@
 自己解决</t>
   </si>
   <si>
+    <t xml:space="preserve">8022QM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">反应概率性开机没有指纹菜单</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MM8068T-B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5产线问题</t>
+  </si>
+  <si>
+    <t xml:space="preserve">反应产线数据上传失败</t>
+  </si>
+  <si>
+    <t xml:space="preserve">更新上传工具</t>
+  </si>
+  <si>
     <t xml:space="preserve">K706G_3846_MITO T85_HYD</t>
   </si>
   <si>
@@ -550,6 +568,15 @@
   </si>
   <si>
     <t xml:space="preserve">检查数据中有其他项目的*.pubkey存在，删掉之后再上传解决</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y89938_V45A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">反应写key失败</t>
+  </si>
+  <si>
+    <t xml:space="preserve">检查是kph ta版本使用版本不对</t>
   </si>
   <si>
     <t xml:space="preserve">3643_LF708_navitel</t>
@@ -642,10 +669,21 @@
 更换最新版tee.bin解决</t>
   </si>
   <si>
+    <t xml:space="preserve">LF713</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8其它问题</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTS测试失败，失败项为
+android.keystore.cts.KeyAttestationTest.testRsaAttestations
+android.keystore.cts.KeyAttestationTest.testEcAttestation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">没有写key导致</t>
+  </si>
+  <si>
     <t xml:space="preserve">T758-8071C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5产线问题</t>
   </si>
   <si>
     <t xml:space="preserve">工厂写号失败，不能恢复出厂设置</t>
@@ -697,9 +735,6 @@
   </si>
   <si>
     <t xml:space="preserve">C719-8045C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8其它问题</t>
   </si>
   <si>
     <t xml:space="preserve">在工厂使用MES系统写号后不能恢复
@@ -954,6 +989,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86046511627907"/>
+  </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1" t="s">
@@ -1048,18 +1086,19 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.506976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.4744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.4883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.7767441860465"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.1627906976744"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.1209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.8697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.8837209302326"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1237,21 +1276,41 @@
       <c r="G8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="35.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="n">
+        <v>20180906</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+    <row r="10" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>20180906</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>20180906</v>
+      </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,17 +1356,18 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.3953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.1906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.5302325581395"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.4883720930233"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.2558139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.4883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="61.0372093023256"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="88.1116279069768"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,7 +1395,7 @@
     </row>
     <row r="2" customFormat="false" ht="42" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>20180524</v>
@@ -1344,10 +1404,10 @@
         <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F2" s="6" t="n">
         <v>20180524</v>
@@ -1356,19 +1416,19 @@
     </row>
     <row r="3" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>20180601</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>20180601</v>
@@ -1377,7 +1437,7 @@
     </row>
     <row r="4" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>20180605</v>
@@ -1386,10 +1446,10 @@
         <v>31</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>20180608</v>
@@ -1398,19 +1458,19 @@
     </row>
     <row r="5" customFormat="false" ht="44.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>20180620</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>20180620</v>
@@ -1419,19 +1479,19 @@
     </row>
     <row r="6" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>20180619</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>20180619</v>
@@ -1440,19 +1500,19 @@
     </row>
     <row r="7" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>20180620</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>20180621</v>
@@ -1461,19 +1521,19 @@
     </row>
     <row r="8" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>20180622</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>20180622</v>
@@ -1482,7 +1542,7 @@
     </row>
     <row r="9" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>20180702</v>
@@ -1491,10 +1551,10 @@
         <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>20180702</v>
@@ -1503,7 +1563,7 @@
     </row>
     <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>20180721</v>
@@ -1512,10 +1572,10 @@
         <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>20180720</v>
@@ -1524,7 +1584,7 @@
     </row>
     <row r="11" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>20180723</v>
@@ -1533,10 +1593,10 @@
         <v>23</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>20180723</v>
@@ -1545,7 +1605,7 @@
     </row>
     <row r="12" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B12" s="3" t="n">
         <v>20180725</v>
@@ -1554,10 +1614,10 @@
         <v>27</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>20180726</v>
@@ -1566,19 +1626,19 @@
     </row>
     <row r="13" customFormat="false" ht="55.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="B13" s="3" t="n">
         <v>20180731</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>20180731</v>
@@ -1587,7 +1647,7 @@
     </row>
     <row r="14" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>20180802</v>
@@ -1596,44 +1656,44 @@
         <v>45</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>20180806</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>20180806</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>20180806</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="40.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>20180807</v>
@@ -1642,39 +1702,58 @@
         <v>31</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>20180809</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>20180816</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="F17" s="0" t="n">
         <v>20180816</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>20180903</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>20180903</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="true" operator="between" prompt="1. 开机问题　如：黑屏问题，重启问题；2. 指纹问题　如：指纹cts测试问题，指纹性能问题，指纹无菜单问题; 3. 性能问题　如：手机卡顿问题 ; 4. Gms测试问题　如：gms相关测试失败问题；5. 产线问题 如：工具对接问题， 工具使用问题； ６．keybox问题 如：如何申请keybox,  如何拆分， 如何写入以及保管问题；７．支付问题；８,其他问题" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C2:C13" type="list">
@@ -1697,20 +1776,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="73.4697674418605"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="48.6093023255814"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.1209302325581"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.6279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.046511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="75.6837209302326"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.0883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.8604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,19 +1818,19 @@
     </row>
     <row r="2" customFormat="false" ht="70.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>20180529</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>20180529</v>
@@ -1759,7 +1839,7 @@
     </row>
     <row r="3" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>20180622</v>
@@ -1768,10 +1848,10 @@
         <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>20180702</v>
@@ -1780,7 +1860,7 @@
     </row>
     <row r="4" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>20180725</v>
@@ -1789,10 +1869,10 @@
         <v>45</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>20180725</v>
@@ -1801,7 +1881,7 @@
     </row>
     <row r="5" customFormat="false" ht="31.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>20180730</v>
@@ -1810,10 +1890,10 @@
         <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>20180730</v>
@@ -1831,10 +1911,10 @@
         <v>31</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>20180806</v>
@@ -1855,7 +1935,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>20180821</v>
@@ -1868,13 +1948,13 @@
         <v>20180822</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>20180822</v>
@@ -1892,10 +1972,10 @@
         <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>20180823</v>
@@ -1911,10 +1991,10 @@
         <v>27</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>20180823</v>
@@ -1932,10 +2012,10 @@
         <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>20180829</v>
@@ -1951,10 +2031,10 @@
         <v>31</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>20180830</v>
@@ -1963,7 +2043,7 @@
     </row>
     <row r="13" customFormat="false" ht="42.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>20180830</v>
@@ -1972,13 +2052,33 @@
         <v>45</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>20180831</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="54.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>20180907</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>20180907</v>
       </c>
     </row>
   </sheetData>
@@ -2011,11 +2111,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.2139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="69.6511627906977"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="88.2372093023256"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.706976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.4139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="71.7441860465116"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="90.9441860465116"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,19 +2144,19 @@
     </row>
     <row r="2" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>20180530</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>20180531</v>
@@ -2064,7 +2165,7 @@
     </row>
     <row r="3" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>20180530</v>
@@ -2073,10 +2174,10 @@
         <v>23</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>20180531</v>
@@ -2085,7 +2186,7 @@
     </row>
     <row r="4" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>20180723</v>
@@ -2094,10 +2195,10 @@
         <v>45</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>20180724</v>
@@ -2106,7 +2207,7 @@
     </row>
     <row r="5" customFormat="false" ht="35.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>20180806</v>
@@ -2115,10 +2216,10 @@
         <v>45</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>20180806</v>
@@ -2127,7 +2228,7 @@
     </row>
     <row r="6" customFormat="false" ht="33.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>20180816</v>
@@ -2136,10 +2237,10 @@
         <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>20180821</v>
@@ -2155,10 +2256,10 @@
         <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>20180823</v>
@@ -2167,16 +2268,16 @@
     </row>
     <row r="8" customFormat="false" ht="37.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>20180829</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -2242,18 +2343,19 @@
   </sheetPr>
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4139534883721"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="98.3255813953488"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.1674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2744186046512"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="101.279069767442"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,19 +2383,19 @@
     </row>
     <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>20180519</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>20180525</v>
@@ -2302,7 +2404,7 @@
     </row>
     <row r="3" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>20180524</v>
@@ -2311,10 +2413,10 @@
         <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>20180524</v>
@@ -2323,7 +2425,7 @@
     </row>
     <row r="4" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>20180605</v>
@@ -2332,10 +2434,10 @@
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>20180605</v>
@@ -2344,7 +2446,7 @@
     </row>
     <row r="5" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>20180609</v>
@@ -2353,10 +2455,10 @@
         <v>45</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>20180611</v>
@@ -2365,7 +2467,7 @@
     </row>
     <row r="6" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>20180621</v>
@@ -2374,10 +2476,10 @@
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>20180621</v>
@@ -2386,7 +2488,7 @@
     </row>
     <row r="7" customFormat="false" ht="31.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>20180830</v>
@@ -2395,7 +2497,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -2480,17 +2582,18 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.2418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.3488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="85.6511627906977"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="59.0697674418605"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="88.2372093023256"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,19 +2621,19 @@
     </row>
     <row r="2" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>20180528</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>20180528</v>
@@ -2539,7 +2642,7 @@
     </row>
     <row r="3" customFormat="false" ht="29.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>20180725</v>
@@ -2548,10 +2651,10 @@
         <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>20180725</v>
@@ -2664,19 +2767,19 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.1627906976744"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.9302325581395"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.6418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.6558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.753488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="12.1813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2690,7 +2793,7 @@
         <v>17</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>19</v>
@@ -2704,19 +2807,19 @@
     </row>
     <row r="2" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>20180823</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>20180824</v>
@@ -2727,13 +2830,13 @@
         <v>20180827</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>20180828</v>
@@ -2747,8 +2850,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,标准"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,标准"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>